<commit_message>
Descriptions optimized and versionized
</commit_message>
<xml_diff>
--- a/wordpress/wp-content/themes/bsawesome/inc/configurator/options.xlsx
+++ b/wordpress/wp-content/themes/bsawesome/inc/configurator/options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\imabidin\badspiegel\wordpress\wp-content\themes\bsawesome\inc\configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B2543F-80B7-42E4-BD0A-4C7D3D4CE5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFDE45F-E3DF-48F8-A550-15CD78C412DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="3360" windowWidth="28800" windowHeight="14565" xr2:uid="{8A239F44-A77C-4AD1-88FA-34A33C3D37BF}"/>
+    <workbookView xWindow="3975" yWindow="4050" windowWidth="28800" windowHeight="14565" xr2:uid="{8A239F44-A77C-4AD1-88FA-34A33C3D37BF}"/>
   </bookViews>
   <sheets>
     <sheet name="options" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3109" uniqueCount="1355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3109" uniqueCount="1357">
   <si>
     <t>option</t>
   </si>
@@ -3109,9 +3109,6 @@
     <t>stromanschluss</t>
   </si>
   <si>
-    <t>dekor-muster</t>
-  </si>
-  <si>
     <t>design-front-buendig</t>
   </si>
   <si>
@@ -3943,12 +3940,6 @@
     <t>masse/breite-oben</t>
   </si>
   <si>
-    <t>masse/hoehe-unten</t>
-  </si>
-  <si>
-    <t>masse/hoehe-oben</t>
-  </si>
-  <si>
     <t>anschluesse/1steckdose</t>
   </si>
   <si>
@@ -4106,6 +4097,21 @@
   </si>
   <si>
     <t>Höhe rechts in mm</t>
+  </si>
+  <si>
+    <t>masse/hoehe-links</t>
+  </si>
+  <si>
+    <t>masse/hoehe-rechts</t>
+  </si>
+  <si>
+    <t>dekor/korpus</t>
+  </si>
+  <si>
+    <t>dekor/front</t>
+  </si>
+  <si>
+    <t>dekor/muster</t>
   </si>
 </sst>
 </file>
@@ -5106,10 +5112,10 @@
   <dimension ref="A1:V247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q13" sqref="Q13:Q14"/>
+      <selection pane="bottomRight" activeCell="Q90" sqref="Q90:Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5245,7 +5251,7 @@
         <v>127</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>118</v>
@@ -5287,7 +5293,7 @@
         <v>128</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>119</v>
@@ -5329,7 +5335,7 @@
         <v>129</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>120</v>
@@ -5371,7 +5377,7 @@
         <v>130</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>121</v>
@@ -5425,7 +5431,7 @@
         <v>133</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="R12" s="5" t="s">
         <v>801</v>
@@ -5474,7 +5480,7 @@
         <v>781</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="R13" s="5" t="s">
         <v>119</v>
@@ -5523,7 +5529,7 @@
         <v>782</v>
       </c>
       <c r="Q14" s="5" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="R14" s="5" t="s">
         <v>120</v>
@@ -5572,7 +5578,7 @@
         <v>773</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="R15" s="5" t="s">
         <v>800</v>
@@ -6093,7 +6099,7 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>125</v>
@@ -6127,7 +6133,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
@@ -6188,7 +6194,7 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>650</v>
@@ -6217,7 +6223,7 @@
         <v>31</v>
       </c>
       <c r="P49" s="5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="R49" s="11"/>
       <c r="S49" s="11"/>
@@ -6229,7 +6235,7 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>650</v>
@@ -6258,7 +6264,7 @@
         <v>31</v>
       </c>
       <c r="P50" s="5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="R50" s="11"/>
       <c r="S50" s="11"/>
@@ -6270,7 +6276,7 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>650</v>
@@ -6299,7 +6305,7 @@
         <v>31</v>
       </c>
       <c r="P51" s="5" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="R51" s="11"/>
       <c r="S51" s="11"/>
@@ -6344,7 +6350,7 @@
         <v>585</v>
       </c>
       <c r="P54" s="5" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="R54" s="5" t="s">
         <v>837</v>
@@ -6353,10 +6359,10 @@
         <v>1371</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="U54" s="5" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="56" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -6394,7 +6400,7 @@
         <v>41</v>
       </c>
       <c r="P57" s="5" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="R57" s="11"/>
       <c r="S57" s="11"/>
@@ -6432,7 +6438,7 @@
         <v>41</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="R58" s="5" t="s">
         <v>877</v>
@@ -6441,10 +6447,10 @@
         <v>1371</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="U58" s="5" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="60" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -6482,7 +6488,7 @@
         <v>504</v>
       </c>
       <c r="P61" s="5" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="R61" s="11"/>
       <c r="S61" s="11"/>
@@ -6520,7 +6526,7 @@
         <v>503</v>
       </c>
       <c r="P62" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="R62" s="11"/>
       <c r="S62" s="11"/>
@@ -6565,10 +6571,10 @@
         <v>37</v>
       </c>
       <c r="P65" s="5" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="Q65" s="5" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
       <c r="R65" s="11"/>
       <c r="S65" s="11"/>
@@ -6602,16 +6608,16 @@
         <v>31</v>
       </c>
       <c r="O66" s="5" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
       <c r="P66" s="5" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="Q66" s="5" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="R66" s="5" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
       <c r="S66" s="11"/>
       <c r="T66" s="11"/>
@@ -6644,16 +6650,16 @@
         <v>32</v>
       </c>
       <c r="O67" s="5" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="Q67" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="R67" s="5" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
       <c r="S67" s="11"/>
       <c r="T67" s="11"/>
@@ -6686,16 +6692,16 @@
         <v>33</v>
       </c>
       <c r="O68" s="5" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
       <c r="P68" s="5" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="Q68" s="5" t="s">
-        <v>1300</v>
+        <v>1352</v>
       </c>
       <c r="R68" s="5" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
       <c r="S68" s="11"/>
       <c r="T68" s="11"/>
@@ -6728,16 +6734,16 @@
         <v>34</v>
       </c>
       <c r="O69" s="5" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
       <c r="P69" s="5" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="Q69" s="5" t="s">
-        <v>1301</v>
+        <v>1353</v>
       </c>
       <c r="R69" s="5" t="s">
-        <v>1350</v>
+        <v>1347</v>
       </c>
       <c r="S69" s="11"/>
       <c r="T69" s="11"/>
@@ -6785,10 +6791,10 @@
         <v>43</v>
       </c>
       <c r="P72" s="5" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="Q72" s="5" t="s">
-        <v>1335</v>
+        <v>1332</v>
       </c>
       <c r="R72" s="11"/>
       <c r="S72" s="11"/>
@@ -6863,10 +6869,10 @@
         <v>45</v>
       </c>
       <c r="P74" s="5" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="Q74" s="5" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="R74" s="5" t="s">
         <v>846</v>
@@ -6948,7 +6954,7 @@
         <v>849</v>
       </c>
       <c r="Q78" s="5" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
       <c r="R78" s="11"/>
       <c r="S78" s="11"/>
@@ -6989,7 +6995,7 @@
         <v>850</v>
       </c>
       <c r="Q79" s="5" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
       <c r="R79" s="5" t="s">
         <v>847</v>
@@ -7023,10 +7029,10 @@
         <v>50</v>
       </c>
       <c r="P80" s="5" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="Q80" s="5" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
       <c r="R80" s="11"/>
       <c r="S80" s="11"/>
@@ -7062,10 +7068,10 @@
         <v>50</v>
       </c>
       <c r="P81" s="5" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="Q81" s="5" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
       <c r="R81" s="11"/>
       <c r="S81" s="11"/>
@@ -7281,7 +7287,7 @@
         <v>150</v>
       </c>
       <c r="Q90" s="5" t="s">
-        <v>892</v>
+        <v>1354</v>
       </c>
       <c r="R90" s="11"/>
       <c r="S90" s="11"/>
@@ -7322,7 +7328,7 @@
         <v>150</v>
       </c>
       <c r="Q91" s="5" t="s">
-        <v>893</v>
+        <v>1355</v>
       </c>
       <c r="R91" s="11"/>
       <c r="S91" s="11"/>
@@ -7366,7 +7372,7 @@
         <v>150</v>
       </c>
       <c r="Q92" s="5" t="s">
-        <v>1022</v>
+        <v>1356</v>
       </c>
       <c r="R92" s="11"/>
       <c r="S92" s="11"/>
@@ -7408,7 +7414,7 @@
         <v>2500</v>
       </c>
       <c r="O95" s="5" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="P95" s="5" t="s">
         <v>987</v>
@@ -7462,7 +7468,7 @@
         <v>760</v>
       </c>
       <c r="Q98" s="5" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="R98" s="11"/>
       <c r="S98" s="11"/>
@@ -7510,7 +7516,7 @@
         <v>765</v>
       </c>
       <c r="Q101" s="5" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="R101" s="5" t="s">
         <v>897</v>
@@ -7547,7 +7553,7 @@
         <v>761</v>
       </c>
       <c r="Q102" s="5" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="R102" s="11"/>
       <c r="S102" s="11"/>
@@ -7586,7 +7592,7 @@
         <v>762</v>
       </c>
       <c r="Q103" s="5" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="R103" s="11"/>
       <c r="S103" s="11"/>
@@ -7625,7 +7631,7 @@
         <v>824</v>
       </c>
       <c r="Q104" s="5" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="R104" s="11"/>
       <c r="S104" s="11"/>
@@ -7641,7 +7647,7 @@
         <v>126</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
@@ -7708,7 +7714,7 @@
         <v>825</v>
       </c>
       <c r="Q108" s="5" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
       <c r="R108" s="5" t="s">
         <v>666</v>
@@ -7745,7 +7751,7 @@
         <v>766</v>
       </c>
       <c r="Q109" s="5" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
       <c r="R109" s="11"/>
       <c r="S109" s="11"/>
@@ -7784,7 +7790,7 @@
         <v>761</v>
       </c>
       <c r="Q110" s="5" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="R110" s="11"/>
       <c r="S110" s="11"/>
@@ -7823,7 +7829,7 @@
         <v>762</v>
       </c>
       <c r="Q111" s="5" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="R111" s="11"/>
       <c r="S111" s="11"/>
@@ -7839,7 +7845,7 @@
         <v>126</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
@@ -7906,7 +7912,7 @@
         <v>759</v>
       </c>
       <c r="Q115" s="5" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="R115" s="5" t="s">
         <v>655</v>
@@ -7943,7 +7949,7 @@
         <v>764</v>
       </c>
       <c r="Q116" s="5" t="s">
-        <v>1323</v>
+        <v>1320</v>
       </c>
       <c r="S116" s="11"/>
       <c r="T116" s="11"/>
@@ -7981,7 +7987,7 @@
         <v>761</v>
       </c>
       <c r="Q117" s="5" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="R117" s="11"/>
       <c r="S117" s="11"/>
@@ -8020,7 +8026,7 @@
         <v>762</v>
       </c>
       <c r="Q118" s="5" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="R118" s="11"/>
       <c r="S118" s="11"/>
@@ -8036,7 +8042,7 @@
         <v>126</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
@@ -8120,7 +8126,7 @@
         <v>125</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
@@ -8143,7 +8149,7 @@
         <v>616</v>
       </c>
       <c r="Q123" s="5" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="S123" s="11"/>
       <c r="T123" s="11"/>
@@ -8158,7 +8164,7 @@
         <v>125</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
@@ -8181,7 +8187,7 @@
         <v>616</v>
       </c>
       <c r="Q124" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="S124" s="11"/>
       <c r="T124" s="11"/>
@@ -8196,7 +8202,7 @@
         <v>125</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
@@ -8219,7 +8225,7 @@
         <v>616</v>
       </c>
       <c r="Q125" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="S125" s="11"/>
       <c r="T125" s="11"/>
@@ -8234,7 +8240,7 @@
         <v>125</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
@@ -8257,7 +8263,7 @@
         <v>616</v>
       </c>
       <c r="Q126" s="5" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="S126" s="11"/>
       <c r="T126" s="11"/>
@@ -8272,7 +8278,7 @@
         <v>125</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
@@ -8295,7 +8301,7 @@
         <v>616</v>
       </c>
       <c r="Q127" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="S127" s="11"/>
       <c r="T127" s="11"/>
@@ -8310,7 +8316,7 @@
         <v>125</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
@@ -8333,7 +8339,7 @@
         <v>616</v>
       </c>
       <c r="Q128" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="S128" s="11"/>
       <c r="T128" s="11"/>
@@ -8348,7 +8354,7 @@
         <v>125</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
@@ -8374,7 +8380,7 @@
         <v>616</v>
       </c>
       <c r="Q129" s="5" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="S129" s="11"/>
       <c r="T129" s="11"/>
@@ -8389,7 +8395,7 @@
         <v>125</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
@@ -8415,7 +8421,7 @@
         <v>616</v>
       </c>
       <c r="Q130" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="S130" s="11"/>
       <c r="T130" s="11"/>
@@ -8430,7 +8436,7 @@
         <v>125</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
@@ -8456,7 +8462,7 @@
         <v>616</v>
       </c>
       <c r="Q131" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="S131" s="11"/>
       <c r="T131" s="11"/>
@@ -8559,7 +8565,7 @@
         <v>678</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
@@ -8598,7 +8604,7 @@
         <v>678</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
@@ -8633,7 +8639,7 @@
         <v>678</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
@@ -8668,7 +8674,7 @@
         <v>678</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
@@ -8703,7 +8709,7 @@
         <v>678</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
@@ -8738,7 +8744,7 @@
         <v>678</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
@@ -8773,7 +8779,7 @@
         <v>678</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
@@ -8859,7 +8865,7 @@
         <v>651</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
@@ -8882,7 +8888,7 @@
         <v>478</v>
       </c>
       <c r="Q150" s="5" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="R150" s="11"/>
       <c r="S150" s="11"/>
@@ -8892,13 +8898,13 @@
     </row>
     <row r="151" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
@@ -8921,7 +8927,7 @@
         <v>479</v>
       </c>
       <c r="Q151" s="5" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="S151" s="11"/>
       <c r="T151" s="11"/>
@@ -8930,13 +8936,13 @@
     </row>
     <row r="152" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>125</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
@@ -8959,7 +8965,7 @@
         <v>480</v>
       </c>
       <c r="Q152" s="5" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="S152" s="11"/>
       <c r="T152" s="11"/>
@@ -8981,7 +8987,7 @@
         <v>650</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
@@ -9004,7 +9010,7 @@
         <v>491</v>
       </c>
       <c r="Q155" s="5" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R155" s="5" t="s">
         <v>672</v>
@@ -9025,7 +9031,7 @@
         <v>650</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
@@ -9048,7 +9054,7 @@
         <v>481</v>
       </c>
       <c r="Q158" s="5" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="160" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -9066,7 +9072,7 @@
         <v>650</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
@@ -9089,7 +9095,7 @@
         <v>141</v>
       </c>
       <c r="Q161" s="5" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="R161" s="5" t="s">
         <v>667</v>
@@ -9103,7 +9109,7 @@
         <v>651</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
@@ -9126,7 +9132,7 @@
         <v>482</v>
       </c>
       <c r="Q162" s="5" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="R162" s="5" t="s">
         <v>667</v>
@@ -9185,7 +9191,7 @@
         <v>651</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
@@ -9221,7 +9227,7 @@
         <v>609</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
@@ -9259,7 +9265,7 @@
         <v>609</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
@@ -9394,7 +9400,7 @@
         <v>651</v>
       </c>
       <c r="C175" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D175" s="11"/>
       <c r="E175" s="11"/>
@@ -9417,7 +9423,7 @@
         <v>484</v>
       </c>
       <c r="Q175" s="5" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="R175" s="11"/>
       <c r="S175" s="11"/>
@@ -9507,7 +9513,7 @@
         <v>138</v>
       </c>
       <c r="Q181" s="5" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="R181" s="5" t="s">
         <v>663</v>
@@ -9516,7 +9522,7 @@
         <v>2000</v>
       </c>
       <c r="U181" s="5" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.25">
@@ -9550,7 +9556,7 @@
         <v>138</v>
       </c>
       <c r="Q182" s="5" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="R182" s="5" t="s">
         <v>663</v>
@@ -9559,7 +9565,7 @@
         <v>2038</v>
       </c>
       <c r="U182" s="5" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.25">
@@ -9593,7 +9599,7 @@
         <v>138</v>
       </c>
       <c r="Q183" s="5" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="R183" s="5" t="s">
         <v>663</v>
@@ -9602,7 +9608,7 @@
         <v>2046</v>
       </c>
       <c r="U183" s="5" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.25">
@@ -9636,7 +9642,7 @@
         <v>138</v>
       </c>
       <c r="Q184" s="5" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="R184" s="5" t="s">
         <v>663</v>
@@ -9645,7 +9651,7 @@
         <v>2008</v>
       </c>
       <c r="U184" s="5" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.25">
@@ -9674,7 +9680,7 @@
         <v>138</v>
       </c>
       <c r="Q185" s="5" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="R185" s="5" t="s">
         <v>663</v>
@@ -9683,7 +9689,7 @@
         <v>2008</v>
       </c>
       <c r="U185" s="5" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="187" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -9724,7 +9730,7 @@
         <v>485</v>
       </c>
       <c r="Q188" s="5" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="R188" s="11"/>
       <c r="S188" s="11"/>
@@ -9770,7 +9776,7 @@
         <v>486</v>
       </c>
       <c r="Q191" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R191" s="11"/>
       <c r="S191" s="11"/>
@@ -9809,7 +9815,7 @@
         <v>486</v>
       </c>
       <c r="Q192" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R192" s="11"/>
       <c r="S192" s="11"/>
@@ -9848,7 +9854,7 @@
         <v>486</v>
       </c>
       <c r="Q193" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R193" s="11"/>
       <c r="S193" s="11"/>
@@ -9887,7 +9893,7 @@
         <v>486</v>
       </c>
       <c r="Q194" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R194" s="11"/>
       <c r="S194" s="11"/>
@@ -9926,7 +9932,7 @@
         <v>486</v>
       </c>
       <c r="Q195" s="5" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="R195" s="11"/>
       <c r="S195" s="11"/>
@@ -9949,7 +9955,7 @@
         <v>651</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
@@ -9972,7 +9978,7 @@
         <v>487</v>
       </c>
       <c r="Q198" s="5" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="R198" s="11"/>
       <c r="S198" s="11"/>
@@ -9995,7 +10001,7 @@
         <v>651</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
@@ -10018,7 +10024,7 @@
         <v>483</v>
       </c>
       <c r="Q201" s="5" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="R201" s="11"/>
       <c r="S201" s="11"/>
@@ -10034,7 +10040,7 @@
         <v>609</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D202" s="11"/>
       <c r="E202" s="11"/>
@@ -10069,7 +10075,7 @@
         <v>609</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D203" s="11"/>
       <c r="E203" s="11"/>
@@ -10569,7 +10575,7 @@
         <v>651</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D221" s="11"/>
       <c r="E221" s="11"/>
@@ -10593,7 +10599,7 @@
         <v>469</v>
       </c>
       <c r="Q221" s="5" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="R221" s="11"/>
       <c r="S221" s="11"/>
@@ -10609,7 +10615,7 @@
         <v>651</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D222" s="11"/>
       <c r="E222" s="11"/>
@@ -10633,7 +10639,7 @@
         <v>468</v>
       </c>
       <c r="Q222" s="5" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="R222" s="11"/>
       <c r="S222" s="11"/>
@@ -10697,7 +10703,7 @@
         <v>651</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D226" s="11"/>
       <c r="E226" s="11"/>
@@ -10724,7 +10730,7 @@
         <v>466</v>
       </c>
       <c r="Q226" s="5" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="R226" s="11"/>
       <c r="S226" s="11"/>
@@ -10740,7 +10746,7 @@
         <v>651</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D227" s="11"/>
       <c r="E227" s="11"/>
@@ -10767,7 +10773,7 @@
         <v>467</v>
       </c>
       <c r="Q227" s="5" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="R227" s="11"/>
       <c r="S227" s="11"/>
@@ -10828,7 +10834,7 @@
         <v>651</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D231" s="11"/>
       <c r="E231" s="11"/>
@@ -10852,7 +10858,7 @@
         <v>146</v>
       </c>
       <c r="Q231" s="5" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="R231" s="11"/>
       <c r="S231" s="11"/>
@@ -10868,7 +10874,7 @@
         <v>651</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D232" s="11"/>
       <c r="E232" s="11"/>
@@ -10892,7 +10898,7 @@
         <v>146</v>
       </c>
       <c r="Q232" s="5" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="R232" s="11"/>
       <c r="S232" s="11"/>
@@ -10908,7 +10914,7 @@
         <v>651</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D233" s="11"/>
       <c r="E233" s="11"/>
@@ -10932,7 +10938,7 @@
         <v>463</v>
       </c>
       <c r="Q233" s="5" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="R233" s="11"/>
       <c r="S233" s="11"/>
@@ -10948,7 +10954,7 @@
         <v>651</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D234" s="11"/>
       <c r="E234" s="11"/>
@@ -10972,7 +10978,7 @@
         <v>462</v>
       </c>
       <c r="Q234" s="5" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="R234" s="11"/>
       <c r="S234" s="11"/>
@@ -10995,7 +11001,7 @@
         <v>650</v>
       </c>
       <c r="C237" s="5" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D237" s="11"/>
       <c r="E237" s="11"/>
@@ -11019,7 +11025,7 @@
         <v>465</v>
       </c>
       <c r="Q237" s="5" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="R237" s="5" t="s">
         <v>658</v>
@@ -11033,7 +11039,7 @@
         <v>651</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D238" s="11"/>
       <c r="E238" s="11"/>
@@ -11057,7 +11063,7 @@
         <v>464</v>
       </c>
       <c r="Q238" s="5" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R238" s="11"/>
       <c r="S238" s="11"/>
@@ -11188,7 +11194,7 @@
         <v>1021</v>
       </c>
       <c r="R247" s="5" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
   </sheetData>
@@ -11260,109 +11266,109 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D5">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B6">
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D6">
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B7">
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D7">
         <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B8">
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D8">
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -11374,12 +11380,12 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -11391,12 +11397,12 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B14">
         <v>20</v>
@@ -11408,7 +11414,7 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -11433,10 +11439,10 @@
         <v>1363</v>
       </c>
       <c r="F17" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G17" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -11456,10 +11462,10 @@
         <v>1365</v>
       </c>
       <c r="F18" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G18" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -11479,10 +11485,10 @@
         <v>1367</v>
       </c>
       <c r="F19" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G19" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -11502,10 +11508,10 @@
         <v>1369</v>
       </c>
       <c r="F20" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G20" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -11530,7 +11536,7 @@
         <v>1363</v>
       </c>
       <c r="F23" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -11550,10 +11556,10 @@
         <v>1365</v>
       </c>
       <c r="F24" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G24" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -11573,10 +11579,10 @@
         <v>1367</v>
       </c>
       <c r="F25" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G25" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -11596,10 +11602,10 @@
         <v>1369</v>
       </c>
       <c r="F26" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G26" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -11619,10 +11625,10 @@
         <v>1363</v>
       </c>
       <c r="F27" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G27" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -11642,10 +11648,10 @@
         <v>1365</v>
       </c>
       <c r="F28" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G28" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -11665,10 +11671,10 @@
         <v>1367</v>
       </c>
       <c r="F29" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G29" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -11688,10 +11694,10 @@
         <v>1369</v>
       </c>
       <c r="F30" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G30" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -11991,7 +11997,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -12008,7 +12014,7 @@
         <v>199.99</v>
       </c>
       <c r="F58" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -12025,7 +12031,7 @@
         <v>249.99</v>
       </c>
       <c r="F59" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -12042,7 +12048,7 @@
         <v>619.99</v>
       </c>
       <c r="F60" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -12059,7 +12065,7 @@
         <v>699.99</v>
       </c>
       <c r="F61" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12264,7 +12270,7 @@
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -12281,7 +12287,7 @@
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -12298,7 +12304,7 @@
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -12315,7 +12321,7 @@
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -12332,7 +12338,7 @@
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -12349,7 +12355,7 @@
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -12366,7 +12372,7 @@
         <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -12383,7 +12389,7 @@
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="87" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12408,7 +12414,7 @@
         <v>2114</v>
       </c>
       <c r="F88" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -12428,7 +12434,7 @@
         <v>2112</v>
       </c>
       <c r="F89" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -12448,7 +12454,7 @@
         <v>2110</v>
       </c>
       <c r="F90" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -12468,7 +12474,7 @@
         <v>2106</v>
       </c>
       <c r="F91" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -12488,7 +12494,7 @@
         <v>2102</v>
       </c>
       <c r="F92" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -12508,7 +12514,7 @@
         <v>2104</v>
       </c>
       <c r="F93" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="95" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12577,7 +12583,7 @@
         <v>1451</v>
       </c>
       <c r="F102" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -12597,7 +12603,7 @@
         <v>1453</v>
       </c>
       <c r="F103" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="105" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12622,7 +12628,7 @@
         <v>1159</v>
       </c>
       <c r="F106" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -12642,7 +12648,7 @@
         <v>1161</v>
       </c>
       <c r="F107" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12667,7 +12673,7 @@
         <v>1275</v>
       </c>
       <c r="F110" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -12687,7 +12693,7 @@
         <v>2274</v>
       </c>
       <c r="F111" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -12707,7 +12713,7 @@
         <v>2278</v>
       </c>
       <c r="F112" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -12727,7 +12733,7 @@
         <v>1285</v>
       </c>
       <c r="F113" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -12747,7 +12753,7 @@
         <v>1265</v>
       </c>
       <c r="F114" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -12767,7 +12773,7 @@
         <v>1269</v>
       </c>
       <c r="F115" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="117" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12792,7 +12798,7 @@
         <v>1265</v>
       </c>
       <c r="F118" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -12812,7 +12818,7 @@
         <v>1291</v>
       </c>
       <c r="F119" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="121" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12837,7 +12843,7 @@
         <v>1289</v>
       </c>
       <c r="F122" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -12857,7 +12863,7 @@
         <v>1287</v>
       </c>
       <c r="F123" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -12877,7 +12883,7 @@
         <v>1279</v>
       </c>
       <c r="F124" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -12897,7 +12903,7 @@
         <v>1283</v>
       </c>
       <c r="F125" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -12917,7 +12923,7 @@
         <v>1281</v>
       </c>
       <c r="F126" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -12937,7 +12943,7 @@
         <v>1285</v>
       </c>
       <c r="F127" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="129" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12962,7 +12968,7 @@
         <v>2280</v>
       </c>
       <c r="F130" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -12982,7 +12988,7 @@
         <v>2270</v>
       </c>
       <c r="F131" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -13002,7 +13008,7 @@
         <v>2276</v>
       </c>
       <c r="F132" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -13022,7 +13028,7 @@
         <v>2272</v>
       </c>
       <c r="F133" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="135" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -13673,7 +13679,7 @@
         <v>2182</v>
       </c>
       <c r="F178" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
@@ -14276,7 +14282,7 @@
         <v>2282</v>
       </c>
       <c r="F218" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -14296,7 +14302,7 @@
         <v>2284</v>
       </c>
       <c r="F219" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -14316,7 +14322,7 @@
         <v>2286</v>
       </c>
       <c r="F220" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -14336,7 +14342,7 @@
         <v>2288</v>
       </c>
       <c r="F221" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -14356,7 +14362,7 @@
         <v>2290</v>
       </c>
       <c r="F222" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
@@ -14376,7 +14382,7 @@
         <v>2292</v>
       </c>
       <c r="F223" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
@@ -14396,7 +14402,7 @@
         <v>2294</v>
       </c>
       <c r="F224" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="226" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -14421,7 +14427,7 @@
         <v>1167</v>
       </c>
       <c r="F227" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -14441,7 +14447,7 @@
         <v>1169</v>
       </c>
       <c r="F228" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
@@ -14461,7 +14467,7 @@
         <v>2064</v>
       </c>
       <c r="F229" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
@@ -14481,7 +14487,7 @@
         <v>1181</v>
       </c>
       <c r="F230" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
@@ -14501,7 +14507,7 @@
         <v>1191</v>
       </c>
       <c r="F231" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
@@ -14521,7 +14527,7 @@
         <v>1175</v>
       </c>
       <c r="F232" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
@@ -14541,7 +14547,7 @@
         <v>2066</v>
       </c>
       <c r="F233" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="235" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -14566,7 +14572,7 @@
         <v>1191</v>
       </c>
       <c r="F236" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -14586,7 +14592,7 @@
         <v>1189</v>
       </c>
       <c r="F237" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="239" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -14611,7 +14617,7 @@
         <v>1187</v>
       </c>
       <c r="F240" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
@@ -14631,7 +14637,7 @@
         <v>1185</v>
       </c>
       <c r="F241" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
@@ -14651,7 +14657,7 @@
         <v>1177</v>
       </c>
       <c r="F242" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
@@ -14671,7 +14677,7 @@
         <v>1181</v>
       </c>
       <c r="F243" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
@@ -14691,7 +14697,7 @@
         <v>1179</v>
       </c>
       <c r="F244" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
@@ -14711,7 +14717,7 @@
         <v>1183</v>
       </c>
       <c r="F245" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="247" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -14781,7 +14787,7 @@
         <v>1527</v>
       </c>
       <c r="F252" t="s">
-        <v>1302</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.25">
@@ -14801,7 +14807,7 @@
         <v>2352</v>
       </c>
       <c r="F253" t="s">
-        <v>1303</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.25">
@@ -14821,7 +14827,7 @@
         <v>2350</v>
       </c>
       <c r="F254" t="s">
-        <v>1304</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.25">
@@ -14841,7 +14847,7 @@
         <v>2354</v>
       </c>
       <c r="F255" t="s">
-        <v>1305</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
@@ -14861,7 +14867,7 @@
         <v>2348</v>
       </c>
       <c r="F256" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
@@ -14881,7 +14887,7 @@
         <v>1531</v>
       </c>
       <c r="F257" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
@@ -14895,7 +14901,7 @@
         <v>119</v>
       </c>
       <c r="F258" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="260" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -14917,7 +14923,7 @@
         <v>0</v>
       </c>
       <c r="F261" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
       <c r="H261" t="s">
         <v>166</v>
@@ -14937,7 +14943,7 @@
         <v>0</v>
       </c>
       <c r="F262" t="s">
-        <v>1310</v>
+        <v>1307</v>
       </c>
       <c r="H262" t="s">
         <v>166</v>
@@ -14957,7 +14963,7 @@
         <v>0</v>
       </c>
       <c r="F263" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
       <c r="H263" t="s">
         <v>166</v>
@@ -14977,7 +14983,7 @@
         <v>0</v>
       </c>
       <c r="F264" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
       <c r="H264" t="s">
         <v>532</v>
@@ -14997,7 +15003,7 @@
         <v>0</v>
       </c>
       <c r="F265" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
       <c r="H265" t="s">
         <v>532</v>
@@ -15017,7 +15023,7 @@
         <v>0</v>
       </c>
       <c r="F266" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
       <c r="H266" t="s">
         <v>532</v>
@@ -15037,7 +15043,7 @@
         <v>0</v>
       </c>
       <c r="F267" t="s">
-        <v>1315</v>
+        <v>1312</v>
       </c>
       <c r="H267" t="s">
         <v>532</v>
@@ -15057,7 +15063,7 @@
         <v>0</v>
       </c>
       <c r="F268" t="s">
-        <v>1316</v>
+        <v>1313</v>
       </c>
       <c r="H268" t="s">
         <v>532</v>
@@ -15077,7 +15083,7 @@
         <v>0</v>
       </c>
       <c r="F269" t="s">
-        <v>1317</v>
+        <v>1314</v>
       </c>
       <c r="H269" t="s">
         <v>532</v>
@@ -15097,7 +15103,7 @@
         <v>0</v>
       </c>
       <c r="F270" t="s">
-        <v>1318</v>
+        <v>1315</v>
       </c>
       <c r="H270" t="s">
         <v>532</v>
@@ -15117,7 +15123,7 @@
         <v>0</v>
       </c>
       <c r="F271" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="H271" t="s">
         <v>532</v>
@@ -15137,7 +15143,7 @@
         <v>0</v>
       </c>
       <c r="F272" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
       <c r="H272" t="s">
         <v>532</v>
@@ -15165,7 +15171,7 @@
         <v>1670</v>
       </c>
       <c r="F275" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="H275">
         <v>1670</v>
@@ -15188,7 +15194,7 @@
         <v>1682</v>
       </c>
       <c r="F276" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
@@ -15208,7 +15214,7 @@
         <v>1680</v>
       </c>
       <c r="F277" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
@@ -15228,7 +15234,7 @@
         <v>1674</v>
       </c>
       <c r="F278" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="H278" t="s">
         <v>807</v>
@@ -15251,7 +15257,7 @@
         <v>1672</v>
       </c>
       <c r="F279" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
@@ -15271,7 +15277,7 @@
         <v>1668</v>
       </c>
       <c r="F280" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
@@ -15291,7 +15297,7 @@
         <v>1678</v>
       </c>
       <c r="F281" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="283" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -15311,7 +15317,7 @@
       </c>
       <c r="D284" s="4"/>
       <c r="F284" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.25">
@@ -15326,7 +15332,7 @@
       </c>
       <c r="D285" s="4"/>
       <c r="F285" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="287" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -15633,7 +15639,7 @@
         <v>1387</v>
       </c>
       <c r="F308" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="310" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -15658,7 +15664,7 @@
         <v>1982</v>
       </c>
       <c r="F311" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
@@ -15678,7 +15684,7 @@
         <v>1327</v>
       </c>
       <c r="F312" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="H312" t="s">
         <v>124</v>
@@ -15701,7 +15707,7 @@
         <v>1325</v>
       </c>
       <c r="F313" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="H313" t="s">
         <v>124</v>
@@ -15724,7 +15730,7 @@
         <v>1309</v>
       </c>
       <c r="F314" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="H314" t="s">
         <v>21</v>
@@ -15744,7 +15750,7 @@
         <v>1984</v>
       </c>
       <c r="F315" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H315" t="s">
         <v>124</v>
@@ -15767,7 +15773,7 @@
         <v>1992</v>
       </c>
       <c r="F316" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="H316" t="s">
         <v>21</v>
@@ -15790,7 +15796,7 @@
         <v>1321</v>
       </c>
       <c r="F317" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="H317" t="s">
         <v>21</v>
@@ -15813,7 +15819,7 @@
         <v>1321</v>
       </c>
       <c r="F318" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="H318" t="s">
         <v>429</v>
@@ -15836,7 +15842,7 @@
         <v>1299</v>
       </c>
       <c r="F319" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="H319" t="s">
         <v>429</v>
@@ -15859,7 +15865,7 @@
         <v>1311</v>
       </c>
       <c r="F320" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="H320" t="s">
         <v>429</v>
@@ -15879,7 +15885,7 @@
         <v>1311</v>
       </c>
       <c r="F321" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="H321" t="s">
         <v>429</v>
@@ -15902,7 +15908,7 @@
         <v>1323</v>
       </c>
       <c r="F322" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="H322" t="s">
         <v>429</v>
@@ -15925,7 +15931,7 @@
         <v>1323</v>
       </c>
       <c r="F323" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="H323" t="s">
         <v>429</v>
@@ -15948,7 +15954,7 @@
         <v>1301</v>
       </c>
       <c r="F324" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="H324" t="s">
         <v>429</v>
@@ -15971,7 +15977,7 @@
         <v>1297</v>
       </c>
       <c r="F325" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="H325" t="s">
         <v>32</v>
@@ -15994,7 +16000,7 @@
         <v>1299</v>
       </c>
       <c r="F326" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="H326" t="s">
         <v>32</v>
@@ -16017,7 +16023,7 @@
         <v>1990</v>
       </c>
       <c r="F327" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="H327" t="s">
         <v>32</v>
@@ -16037,7 +16043,7 @@
         <v>0</v>
       </c>
       <c r="F328" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="H328" t="s">
         <v>32</v>
@@ -16062,7 +16068,7 @@
         <v>0</v>
       </c>
       <c r="F331" s="26" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="H331" t="s">
         <v>124</v>
@@ -16082,7 +16088,7 @@
         <v>0</v>
       </c>
       <c r="F332" s="26" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="H332" t="s">
         <v>124</v>
@@ -16102,7 +16108,7 @@
         <v>0</v>
       </c>
       <c r="F333" s="26" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="H333" t="s">
         <v>124</v>
@@ -16122,7 +16128,7 @@
         <v>0</v>
       </c>
       <c r="F334" s="26" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="H334" t="s">
         <v>124</v>
@@ -16142,7 +16148,7 @@
         <v>0</v>
       </c>
       <c r="F335" s="26" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="H335" t="s">
         <v>124</v>
@@ -16162,7 +16168,7 @@
         <v>0</v>
       </c>
       <c r="F336" s="26" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="H336" t="s">
         <v>124</v>
@@ -16182,7 +16188,7 @@
         <v>0</v>
       </c>
       <c r="F337" s="26" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="H337" t="s">
         <v>124</v>
@@ -16202,7 +16208,7 @@
         <v>0</v>
       </c>
       <c r="F338" s="26" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="H338" t="s">
         <v>21</v>
@@ -16225,7 +16231,7 @@
         <v>0</v>
       </c>
       <c r="F339" s="26" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="H339" t="s">
         <v>21</v>
@@ -16248,7 +16254,7 @@
         <v>0</v>
       </c>
       <c r="F340" s="26" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="H340" t="s">
         <v>21</v>
@@ -16271,7 +16277,7 @@
         <v>0</v>
       </c>
       <c r="F341" s="26" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="H341" t="s">
         <v>21</v>
@@ -16294,7 +16300,7 @@
         <v>0</v>
       </c>
       <c r="F342" s="26" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="H342" t="s">
         <v>21</v>
@@ -16317,7 +16323,7 @@
         <v>0</v>
       </c>
       <c r="F343" s="26" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="H343" t="s">
         <v>21</v>
@@ -16340,7 +16346,7 @@
         <v>0</v>
       </c>
       <c r="F344" s="26" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="H344" t="s">
         <v>21</v>
@@ -16363,7 +16369,7 @@
         <v>0</v>
       </c>
       <c r="F345" s="26" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="H345" t="s">
         <v>21</v>
@@ -16386,7 +16392,7 @@
         <v>0</v>
       </c>
       <c r="F346" s="26" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="H346" t="s">
         <v>21</v>
@@ -16414,7 +16420,7 @@
         <v>0</v>
       </c>
       <c r="F349" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.25">
@@ -16431,7 +16437,7 @@
         <v>129</v>
       </c>
       <c r="F350" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.25">
@@ -16448,7 +16454,7 @@
         <v>79</v>
       </c>
       <c r="F351" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="353" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -16473,7 +16479,7 @@
         <v>1227</v>
       </c>
       <c r="F354" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="I354" t="s">
         <v>769</v>
@@ -16496,7 +16502,7 @@
         <v>1221</v>
       </c>
       <c r="F355" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="I355" t="s">
         <v>770</v>
@@ -16519,7 +16525,7 @@
         <v>1219</v>
       </c>
       <c r="F356" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="I356" t="s">
         <v>771</v>
@@ -16542,7 +16548,7 @@
         <v>1223</v>
       </c>
       <c r="F357" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="I357" t="s">
         <v>770</v>
@@ -16565,7 +16571,7 @@
         <v>2052</v>
       </c>
       <c r="F358" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="I358" t="s">
         <v>772</v>
@@ -16588,7 +16594,7 @@
         <v>2056</v>
       </c>
       <c r="F360" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.25">
@@ -16608,7 +16614,7 @@
         <v>2030</v>
       </c>
       <c r="F361" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.25">
@@ -16628,7 +16634,7 @@
         <v>2026</v>
       </c>
       <c r="F362" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.25">
@@ -16648,7 +16654,7 @@
         <v>2036</v>
       </c>
       <c r="F363" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.25">
@@ -16668,7 +16674,7 @@
         <v>2028</v>
       </c>
       <c r="F364" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="365" spans="1:9" x14ac:dyDescent="0.25">
@@ -16688,7 +16694,7 @@
         <v>2024</v>
       </c>
       <c r="F365" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.25">
@@ -16708,7 +16714,7 @@
         <v>2054</v>
       </c>
       <c r="F366" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.25">
@@ -16728,7 +16734,7 @@
         <v>2044</v>
       </c>
       <c r="F368" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="370" spans="1:6" x14ac:dyDescent="0.25">
@@ -16748,7 +16754,7 @@
         <v>2002</v>
       </c>
       <c r="F370" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="371" spans="1:6" x14ac:dyDescent="0.25">
@@ -16768,7 +16774,7 @@
         <v>2010</v>
       </c>
       <c r="F371" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="372" spans="1:6" x14ac:dyDescent="0.25">
@@ -16788,7 +16794,7 @@
         <v>2006</v>
       </c>
       <c r="F372" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.25">
@@ -16808,7 +16814,7 @@
         <v>2044</v>
       </c>
       <c r="F374" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="376" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -16833,7 +16839,7 @@
         <v>1670</v>
       </c>
       <c r="F377" s="24" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="378" spans="1:6" x14ac:dyDescent="0.25">
@@ -16853,7 +16859,7 @@
         <v>1682</v>
       </c>
       <c r="F378" s="24" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.25">
@@ -16873,7 +16879,7 @@
         <v>1680</v>
       </c>
       <c r="F379" s="24" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.25">
@@ -16884,7 +16890,7 @@
         <v>4</v>
       </c>
       <c r="C380" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D380">
         <v>159</v>
@@ -16893,7 +16899,7 @@
         <v>1672</v>
       </c>
       <c r="F380" s="24" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.25">
@@ -16913,7 +16919,7 @@
         <v>1668</v>
       </c>
       <c r="F381" s="24" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.25">
@@ -16933,7 +16939,7 @@
         <v>1678</v>
       </c>
       <c r="F382" s="24" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="384" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -16955,7 +16961,7 @@
         <v>0</v>
       </c>
       <c r="F385" s="24" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.25">
@@ -16975,7 +16981,7 @@
         <v>1309</v>
       </c>
       <c r="F386" s="24" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.25">
@@ -16995,7 +17001,7 @@
         <v>1992</v>
       </c>
       <c r="F387" s="24" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="I387" t="s">
         <v>768</v>
@@ -17018,7 +17024,7 @@
         <v>1321</v>
       </c>
       <c r="F388" s="24" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="389" spans="1:9" x14ac:dyDescent="0.25">
@@ -17038,7 +17044,7 @@
         <v>1321</v>
       </c>
       <c r="F389" s="24" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="390" spans="1:9" x14ac:dyDescent="0.25">
@@ -17058,7 +17064,7 @@
         <v>1299</v>
       </c>
       <c r="F390" s="24" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="391" spans="1:9" x14ac:dyDescent="0.25">
@@ -17078,7 +17084,7 @@
         <v>1297</v>
       </c>
       <c r="F391" s="24" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="392" spans="1:9" x14ac:dyDescent="0.25">
@@ -17098,7 +17104,7 @@
         <v>1299</v>
       </c>
       <c r="F392" s="24" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.25">
@@ -17118,7 +17124,7 @@
         <v>1990</v>
       </c>
       <c r="F393" s="24" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.25">
@@ -17135,7 +17141,7 @@
         <v>0</v>
       </c>
       <c r="F394" s="24" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="395" spans="1:9" x14ac:dyDescent="0.25">
@@ -17152,7 +17158,7 @@
         <v>0</v>
       </c>
       <c r="F395" s="24" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="396" spans="1:9" x14ac:dyDescent="0.25">
@@ -17172,7 +17178,7 @@
         <v>1327</v>
       </c>
       <c r="F396" s="24" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="397" spans="1:9" x14ac:dyDescent="0.25">
@@ -17192,7 +17198,7 @@
         <v>1325</v>
       </c>
       <c r="F397" s="24" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="398" spans="1:9" x14ac:dyDescent="0.25">
@@ -17212,7 +17218,7 @@
         <v>1984</v>
       </c>
       <c r="F398" s="24" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="399" spans="1:9" x14ac:dyDescent="0.25">
@@ -17232,7 +17238,7 @@
         <v>1297</v>
       </c>
       <c r="F399" s="24" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="400" spans="1:9" x14ac:dyDescent="0.25">
@@ -17252,7 +17258,7 @@
         <v>1990</v>
       </c>
       <c r="F400" s="24" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.25">
@@ -17269,7 +17275,7 @@
         <v>0</v>
       </c>
       <c r="F401" s="24" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.25">
@@ -17286,7 +17292,7 @@
         <v>0</v>
       </c>
       <c r="F402" s="24" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.25">
@@ -17303,7 +17309,7 @@
         <v>0</v>
       </c>
       <c r="F403" s="24" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.25">
@@ -17320,7 +17326,7 @@
         <v>0</v>
       </c>
       <c r="F404" s="24" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.25">
@@ -17340,7 +17346,7 @@
         <v>1986</v>
       </c>
       <c r="F405" s="24" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="406" spans="1:6" x14ac:dyDescent="0.25">
@@ -17360,7 +17366,7 @@
         <v>1297</v>
       </c>
       <c r="F406" s="24" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="407" spans="1:6" x14ac:dyDescent="0.25">
@@ -17380,7 +17386,7 @@
         <v>1990</v>
       </c>
       <c r="F407" s="24" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="408" spans="1:6" x14ac:dyDescent="0.25">
@@ -17397,7 +17403,7 @@
         <v>0</v>
       </c>
       <c r="F408" s="25" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="409" spans="1:6" x14ac:dyDescent="0.25">
@@ -17414,7 +17420,7 @@
         <v>0</v>
       </c>
       <c r="F409" s="24" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.25">
@@ -17431,7 +17437,7 @@
         <v>0</v>
       </c>
       <c r="F410" s="24" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.25">
@@ -17448,7 +17454,7 @@
         <v>0</v>
       </c>
       <c r="F411" s="24" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="412" spans="1:6" x14ac:dyDescent="0.25">
@@ -17468,7 +17474,7 @@
         <v>1986</v>
       </c>
       <c r="F412" s="24" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="413" spans="1:6" x14ac:dyDescent="0.25">
@@ -17488,7 +17494,7 @@
         <v>1297</v>
       </c>
       <c r="F413" s="24" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="414" spans="1:6" x14ac:dyDescent="0.25">
@@ -17508,7 +17514,7 @@
         <v>1990</v>
       </c>
       <c r="F414" s="24" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.25">
@@ -17525,7 +17531,7 @@
         <v>0</v>
       </c>
       <c r="F415" s="25" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="416" spans="1:6" x14ac:dyDescent="0.25">
@@ -17542,7 +17548,7 @@
         <v>0</v>
       </c>
       <c r="F416" s="24" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="417" spans="1:8" x14ac:dyDescent="0.25">
@@ -17559,7 +17565,7 @@
         <v>0</v>
       </c>
       <c r="F417" s="24" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="418" spans="1:8" x14ac:dyDescent="0.25">
@@ -17576,7 +17582,7 @@
         <v>0</v>
       </c>
       <c r="F418" s="24" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="419" spans="1:8" x14ac:dyDescent="0.25">
@@ -17596,7 +17602,7 @@
         <v>1986</v>
       </c>
       <c r="F419" s="24" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="420" spans="1:8" x14ac:dyDescent="0.25">
@@ -17616,7 +17622,7 @@
         <v>1297</v>
       </c>
       <c r="F420" s="24" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="421" spans="1:8" x14ac:dyDescent="0.25">
@@ -17636,7 +17642,7 @@
         <v>1990</v>
       </c>
       <c r="F421" s="24" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="422" spans="1:8" x14ac:dyDescent="0.25">
@@ -17653,7 +17659,7 @@
         <v>0</v>
       </c>
       <c r="F422" s="25" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="424" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -17675,7 +17681,7 @@
         <v>0</v>
       </c>
       <c r="F425" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="H425" t="s">
         <v>682</v>
@@ -17695,7 +17701,7 @@
         <v>0</v>
       </c>
       <c r="F426" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="H426" t="s">
         <v>682</v>
@@ -17715,7 +17721,7 @@
         <v>0</v>
       </c>
       <c r="F427" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="H427" t="s">
         <v>682</v>
@@ -17735,7 +17741,7 @@
         <v>0</v>
       </c>
       <c r="F428" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="H428" t="s">
         <v>682</v>
@@ -17755,7 +17761,7 @@
         <v>0</v>
       </c>
       <c r="F429" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="H429" t="s">
         <v>682</v>
@@ -17775,7 +17781,7 @@
         <v>0</v>
       </c>
       <c r="F430" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="H430" t="s">
         <v>682</v>
@@ -17795,7 +17801,7 @@
         <v>0</v>
       </c>
       <c r="F431" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="H431" t="s">
         <v>682</v>
@@ -17815,7 +17821,7 @@
         <v>0</v>
       </c>
       <c r="F432" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="H432" t="s">
         <v>570</v>
@@ -17835,7 +17841,7 @@
         <v>0</v>
       </c>
       <c r="F433" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="H433" t="s">
         <v>570</v>
@@ -17855,7 +17861,7 @@
         <v>0</v>
       </c>
       <c r="F434" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="H434" t="s">
         <v>570</v>
@@ -17875,7 +17881,7 @@
         <v>0</v>
       </c>
       <c r="F435" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="H435" t="s">
         <v>570</v>
@@ -17895,7 +17901,7 @@
         <v>0</v>
       </c>
       <c r="F436" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="H436" t="s">
         <v>570</v>
@@ -17918,7 +17924,7 @@
         <v>1986</v>
       </c>
       <c r="F437" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="H437" t="s">
         <v>681</v>
@@ -17941,7 +17947,7 @@
         <v>1986</v>
       </c>
       <c r="F438" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="H438" t="s">
         <v>681</v>
@@ -17964,7 +17970,7 @@
         <v>1988</v>
       </c>
       <c r="F439" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="H439" t="s">
         <v>681</v>
@@ -17987,7 +17993,7 @@
         <v>1988</v>
       </c>
       <c r="F440" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="H440" t="s">
         <v>681</v>
@@ -18010,7 +18016,7 @@
       </c>
       <c r="D443" s="4"/>
       <c r="F443" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="444" spans="1:8" x14ac:dyDescent="0.25">
@@ -18025,7 +18031,7 @@
       </c>
       <c r="D444" s="4"/>
       <c r="F444" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="446" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -18787,7 +18793,7 @@
         <v>1201</v>
       </c>
       <c r="F498" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="499" spans="1:6" x14ac:dyDescent="0.25">
@@ -18807,7 +18813,7 @@
         <v>1163</v>
       </c>
       <c r="F499" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.25">
@@ -18827,7 +18833,7 @@
         <v>1205</v>
       </c>
       <c r="F500" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.25">
@@ -18847,7 +18853,7 @@
         <v>1207</v>
       </c>
       <c r="F501" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="502" spans="1:6" x14ac:dyDescent="0.25">
@@ -18867,7 +18873,7 @@
         <v>1211</v>
       </c>
       <c r="F502" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="504" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -18892,7 +18898,7 @@
         <v>1211</v>
       </c>
       <c r="F505" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="506" spans="1:6" x14ac:dyDescent="0.25">
@@ -18912,7 +18918,7 @@
         <v>1199</v>
       </c>
       <c r="F506" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="508" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -18937,7 +18943,7 @@
         <v>1213</v>
       </c>
       <c r="F509" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="510" spans="1:6" x14ac:dyDescent="0.25">
@@ -18957,7 +18963,7 @@
         <v>1209</v>
       </c>
       <c r="F510" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="511" spans="1:6" x14ac:dyDescent="0.25">
@@ -18977,7 +18983,7 @@
         <v>1197</v>
       </c>
       <c r="F511" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="512" spans="1:6" x14ac:dyDescent="0.25">
@@ -18997,7 +19003,7 @@
         <v>2096</v>
       </c>
       <c r="F512" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="513" spans="1:9" x14ac:dyDescent="0.25">
@@ -19017,7 +19023,7 @@
         <v>1203</v>
       </c>
       <c r="F513" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="514" spans="1:9" x14ac:dyDescent="0.25">
@@ -19037,7 +19043,7 @@
         <v>1207</v>
       </c>
       <c r="F514" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="516" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -19313,7 +19319,7 @@
         <v>0</v>
       </c>
       <c r="F537" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="538" spans="1:9" x14ac:dyDescent="0.25">
@@ -19333,7 +19339,7 @@
         <v>1309</v>
       </c>
       <c r="F538" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="539" spans="1:9" x14ac:dyDescent="0.25">
@@ -19353,7 +19359,7 @@
         <v>1515</v>
       </c>
       <c r="F539" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="540" spans="1:9" x14ac:dyDescent="0.25">
@@ -19373,7 +19379,7 @@
         <v>1515</v>
       </c>
       <c r="F540" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="542" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -19395,7 +19401,7 @@
         <v>0</v>
       </c>
       <c r="F543" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="I543" t="s">
         <v>670</v>
@@ -19415,7 +19421,7 @@
         <v>0</v>
       </c>
       <c r="F544" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="I544" t="s">
         <v>670</v>
@@ -19435,7 +19441,7 @@
         <v>0</v>
       </c>
       <c r="F545" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="I545" t="s">
         <v>670</v>
@@ -19455,7 +19461,7 @@
         <v>0</v>
       </c>
       <c r="F546" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="I546" t="s">
         <v>670</v>
@@ -19475,7 +19481,7 @@
         <v>0</v>
       </c>
       <c r="F547" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="I547" t="s">
         <v>670</v>
@@ -19495,7 +19501,7 @@
         <v>0</v>
       </c>
       <c r="F548" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="I548" t="s">
         <v>426</v>
@@ -19515,7 +19521,7 @@
         <v>0</v>
       </c>
       <c r="F549" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="I549" t="s">
         <v>426</v>
@@ -19535,7 +19541,7 @@
         <v>0</v>
       </c>
       <c r="F550" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="I550" t="s">
         <v>426</v>
@@ -19647,7 +19653,7 @@
         <v>1670</v>
       </c>
       <c r="F561" s="24" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="562" spans="1:9" x14ac:dyDescent="0.25">
@@ -19667,7 +19673,7 @@
         <v>1682</v>
       </c>
       <c r="F562" s="24" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="563" spans="1:9" x14ac:dyDescent="0.25">
@@ -19687,7 +19693,7 @@
         <v>1680</v>
       </c>
       <c r="F563" s="24" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="564" spans="1:9" x14ac:dyDescent="0.25">
@@ -19698,7 +19704,7 @@
         <v>4</v>
       </c>
       <c r="C564" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D564">
         <v>39.99</v>
@@ -19707,7 +19713,7 @@
         <v>1686</v>
       </c>
       <c r="F564" s="24" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="566" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -19729,7 +19735,7 @@
         <v>0</v>
       </c>
       <c r="F567" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.25">
@@ -19749,7 +19755,7 @@
         <v>1309</v>
       </c>
       <c r="F568" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="569" spans="1:9" x14ac:dyDescent="0.25">
@@ -19769,7 +19775,7 @@
         <v>1321</v>
       </c>
       <c r="F569" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="570" spans="1:9" x14ac:dyDescent="0.25">
@@ -19789,7 +19795,7 @@
         <v>1321</v>
       </c>
       <c r="F570" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="572" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -19811,7 +19817,7 @@
         <v>0</v>
       </c>
       <c r="F573" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="I573" t="s">
         <v>670</v>
@@ -19831,7 +19837,7 @@
         <v>0</v>
       </c>
       <c r="F574" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="I574" t="s">
         <v>670</v>
@@ -19851,7 +19857,7 @@
         <v>0</v>
       </c>
       <c r="F575" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="I575" t="s">
         <v>670</v>
@@ -19871,7 +19877,7 @@
         <v>0</v>
       </c>
       <c r="F576" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="I576" t="s">
         <v>670</v>
@@ -19891,7 +19897,7 @@
         <v>0</v>
       </c>
       <c r="F577" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="I577" t="s">
         <v>670</v>
@@ -19911,7 +19917,7 @@
         <v>0</v>
       </c>
       <c r="F578" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="I578" t="s">
         <v>426</v>
@@ -19931,7 +19937,7 @@
         <v>0</v>
       </c>
       <c r="F579" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="I579" t="s">
         <v>426</v>
@@ -19951,7 +19957,7 @@
         <v>0</v>
       </c>
       <c r="F580" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="I580" t="s">
         <v>426</v>

</xml_diff>